<commit_message>
created new branch with developing pdf generators
</commit_message>
<xml_diff>
--- a/_zakres_modulu_wyp.xlsx
+++ b/_zakres_modulu_wyp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidpylak/Documents/Economic_Indicators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF25D8D-67DA-E145-9524-24A69D9D8D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA899F7C-39A4-6F4B-8FC5-AC3E71E4BF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="11300" windowWidth="33600" windowHeight="20500" xr2:uid="{C2F22BE8-B2FC-B84B-BEB4-D4C7B8307E66}"/>
+    <workbookView xWindow="-33620" yWindow="11300" windowWidth="33600" windowHeight="20500" xr2:uid="{C2F22BE8-B2FC-B84B-BEB4-D4C7B8307E66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1403,7 +1403,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M91" sqref="M91"/>
+      <selection pane="topRight" activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="11" zeroHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Added pdffiles generator and downloading files, fixed registration and bug with creating the raport
</commit_message>
<xml_diff>
--- a/_zakres_modulu_wyp.xlsx
+++ b/_zakres_modulu_wyp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidpylak/Documents/Economic_Indicators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA899F7C-39A4-6F4B-8FC5-AC3E71E4BF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F0B7D5-488E-114C-8BE9-4560993B5779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33620" yWindow="11300" windowWidth="33600" windowHeight="20500" xr2:uid="{C2F22BE8-B2FC-B84B-BEB4-D4C7B8307E66}"/>
+    <workbookView xWindow="13820" yWindow="8300" windowWidth="33600" windowHeight="20500" xr2:uid="{C2F22BE8-B2FC-B84B-BEB4-D4C7B8307E66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1403,7 +1403,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G86" sqref="G86"/>
+      <selection pane="topRight" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="11" zeroHeight="1" x14ac:dyDescent="0.15"/>
@@ -4222,11 +4222,11 @@
         <v>89</v>
       </c>
       <c r="G88" s="80">
-        <f t="shared" ref="G88:H88" si="46">IF(G35=0,0,G13/G35)</f>
+        <f>IF(G35=0,0,G13/G35)</f>
         <v>8.3117546000000004</v>
       </c>
       <c r="H88" s="80">
-        <f t="shared" si="46"/>
+        <f t="shared" ref="G88:H88" si="46">IF(H35=0,0,H13/H35)</f>
         <v>10.859921800000002</v>
       </c>
       <c r="I88" s="80">
@@ -4433,7 +4433,7 @@
       <formula>"słaba"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4" xr:uid="{528CD7B0-1F70-F64B-8C0A-4CC1EC8E39CC}">
       <formula1>"2012,2013,2014,2015,2016,2017,2018,2019,2020,2021,2022,2023,2024,2025"</formula1>
     </dataValidation>

</xml_diff>